<commit_message>
results from fixed syntax in the eqns
</commit_message>
<xml_diff>
--- a/code/equilibria/full_restoration_model_output.xlsx
+++ b/code/equilibria/full_restoration_model_output.xlsx
@@ -386,10 +386,10 @@
         <v>0</v>
       </c>
       <c r="J1">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
       <c r="K1">
-        <v>0</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -415,16 +415,16 @@
         <v>2</v>
       </c>
       <c r="H2">
-        <v>2</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="I2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>2</v>
+        <v>-0.31</v>
       </c>
       <c r="K2">
-        <v>2</v>
+        <v>0.1631969696969697</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -450,16 +450,16 @@
         <v>3</v>
       </c>
       <c r="H3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>0.87012987012987009</v>
       </c>
       <c r="J3">
-        <v>2</v>
+        <v>-0.67</v>
       </c>
       <c r="K3">
-        <v>2</v>
+        <v>-0.25558441558441558</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -1086,10 +1086,10 @@
         <v>0</v>
       </c>
       <c r="J21">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
       <c r="K21">
-        <v>-0.2</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -1115,16 +1115,16 @@
         <v>2</v>
       </c>
       <c r="H22">
-        <v>2</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="I22">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>-0.31</v>
       </c>
       <c r="K22">
-        <v>2</v>
+        <v>-0.29513636363636364</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -1150,16 +1150,16 @@
         <v>3</v>
       </c>
       <c r="H23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I23">
-        <v>2</v>
+        <v>0.61038961038961037</v>
       </c>
       <c r="J23">
-        <v>2</v>
+        <v>-0.47</v>
       </c>
       <c r="K23">
-        <v>2</v>
+        <v>-8.6753246753246749E-2</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -1185,16 +1185,16 @@
         <v>4</v>
       </c>
       <c r="H24">
-        <v>2</v>
+        <v>0.24663978899259212</v>
       </c>
       <c r="I24">
-        <v>2</v>
+        <v>0.26822787085242206</v>
       </c>
       <c r="J24">
-        <v>2</v>
+        <v>5.8681757957998244E-2</v>
       </c>
       <c r="K24">
-        <v>2</v>
+        <v>-0.4008691024602889</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -1786,10 +1786,10 @@
         <v>0</v>
       </c>
       <c r="J41">
-        <v>-0.4</v>
+        <v>0.27</v>
       </c>
       <c r="K41">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
@@ -1815,16 +1815,16 @@
         <v>2</v>
       </c>
       <c r="H42">
-        <v>2</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="I42">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42">
-        <v>2</v>
+        <v>-0.75346969696969701</v>
       </c>
       <c r="K42">
-        <v>2</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -1850,16 +1850,16 @@
         <v>3</v>
       </c>
       <c r="H43">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I43">
-        <v>2</v>
+        <v>0.35064935064935066</v>
       </c>
       <c r="J43">
-        <v>2</v>
+        <v>-0.27</v>
       </c>
       <c r="K43">
-        <v>2</v>
+        <v>8.2077922077922083E-2</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -2486,10 +2486,10 @@
         <v>0</v>
       </c>
       <c r="J61">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
       <c r="K61">
-        <v>0.2</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
@@ -2515,16 +2515,16 @@
         <v>2</v>
       </c>
       <c r="H62">
+        <v>0.5636363636363636</v>
+      </c>
+      <c r="I62">
         <v>0</v>
       </c>
-      <c r="I62">
-        <v>0.66666666666666663</v>
-      </c>
       <c r="J62">
-        <v>-0.7466666666666667</v>
+        <v>-0.31</v>
       </c>
       <c r="K62">
-        <v>-0.2</v>
+        <v>0.27592424242424241</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -2550,16 +2550,16 @@
         <v>3</v>
       </c>
       <c r="H63">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I63">
-        <v>2</v>
+        <v>0.87012987012987009</v>
       </c>
       <c r="J63">
-        <v>2</v>
+        <v>-0.67</v>
       </c>
       <c r="K63">
-        <v>2</v>
+        <v>-0.42961038961038961</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -3186,10 +3186,10 @@
         <v>0</v>
       </c>
       <c r="J81">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
       <c r="K81">
-        <v>0</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
@@ -3215,16 +3215,16 @@
         <v>2</v>
       </c>
       <c r="H82">
-        <v>2</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="I82">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J82">
-        <v>2</v>
+        <v>-0.31</v>
       </c>
       <c r="K82">
-        <v>2</v>
+        <v>-0.18240909090909091</v>
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
@@ -3250,16 +3250,16 @@
         <v>3</v>
       </c>
       <c r="H83">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I83">
-        <v>2</v>
+        <v>0.61038961038961037</v>
       </c>
       <c r="J83">
-        <v>2</v>
+        <v>-0.47</v>
       </c>
       <c r="K83">
-        <v>2</v>
+        <v>-0.20883116883116884</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
@@ -3285,16 +3285,16 @@
         <v>4</v>
       </c>
       <c r="H84">
-        <v>2</v>
+        <v>0.40058392169550094</v>
       </c>
       <c r="I84">
-        <v>2</v>
+        <v>0.10550452125585233</v>
       </c>
       <c r="J84">
-        <v>2</v>
+        <v>7.6629880197777417E-2</v>
       </c>
       <c r="K84">
-        <v>2</v>
+        <v>-0.37818951849730925</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
@@ -3886,10 +3886,10 @@
         <v>0</v>
       </c>
       <c r="J101">
-        <v>-0.22</v>
+        <v>0.27</v>
       </c>
       <c r="K101">
-        <v>-0.2</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
@@ -3915,16 +3915,16 @@
         <v>2</v>
       </c>
       <c r="H102">
-        <v>2</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="I102">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J102">
-        <v>2</v>
+        <v>-0.64074242424242422</v>
       </c>
       <c r="K102">
-        <v>2</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -3950,16 +3950,16 @@
         <v>3</v>
       </c>
       <c r="H103">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I103">
-        <v>2</v>
+        <v>0.35064935064935066</v>
       </c>
       <c r="J103">
-        <v>2</v>
+        <v>-0.27</v>
       </c>
       <c r="K103">
-        <v>2</v>
+        <v>1.1948051948051949E-2</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
@@ -4586,10 +4586,10 @@
         <v>0</v>
       </c>
       <c r="J121">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
       <c r="K121">
-        <v>0.4</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
@@ -4615,16 +4615,16 @@
         <v>2</v>
       </c>
       <c r="H122">
+        <v>0.5636363636363636</v>
+      </c>
+      <c r="I122">
         <v>0</v>
       </c>
-      <c r="I122">
-        <v>0.8</v>
-      </c>
       <c r="J122">
-        <v>-0.85199999999999998</v>
+        <v>-0.31</v>
       </c>
       <c r="K122">
-        <v>-0.4</v>
+        <v>0.38865151515151514</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
@@ -4650,16 +4650,16 @@
         <v>3</v>
       </c>
       <c r="H123">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I123">
-        <v>2</v>
+        <v>0.87012987012987009</v>
       </c>
       <c r="J123">
-        <v>2</v>
+        <v>-0.67</v>
       </c>
       <c r="K123">
-        <v>2</v>
+        <v>-0.60363636363636364</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
@@ -5286,10 +5286,10 @@
         <v>0</v>
       </c>
       <c r="J141">
-        <v>-0.22</v>
+        <v>0.31</v>
       </c>
       <c r="K141">
-        <v>0.2</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
@@ -5315,16 +5315,16 @@
         <v>2</v>
       </c>
       <c r="H142">
+        <v>0.5636363636363636</v>
+      </c>
+      <c r="I142">
         <v>0</v>
       </c>
-      <c r="I142">
-        <v>0.4</v>
-      </c>
       <c r="J142">
-        <v>-0.53600000000000003</v>
+        <v>-0.31</v>
       </c>
       <c r="K142">
-        <v>-0.2</v>
+        <v>-6.9681818181818178E-2</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
@@ -5350,16 +5350,16 @@
         <v>3</v>
       </c>
       <c r="H143">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I143">
-        <v>2</v>
+        <v>0.61038961038961037</v>
       </c>
       <c r="J143">
-        <v>2</v>
+        <v>-0.47</v>
       </c>
       <c r="K143">
-        <v>2</v>
+        <v>-0.33090909090909093</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
@@ -5385,16 +5385,16 @@
         <v>4</v>
       </c>
       <c r="H144">
-        <v>2</v>
+        <v>0.50858141506522803</v>
       </c>
       <c r="I144">
-        <v>2</v>
+        <v>2.883830639440434E-2</v>
       </c>
       <c r="J144">
-        <v>2</v>
+        <v>4.8705559040263018E-2</v>
       </c>
       <c r="K144">
-        <v>2</v>
+        <v>-0.3506308332498298</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
@@ -5986,10 +5986,10 @@
         <v>0</v>
       </c>
       <c r="J161">
-        <v>-0.22</v>
+        <v>0.27</v>
       </c>
       <c r="K161">
-        <v>0</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
@@ -6015,16 +6015,16 @@
         <v>2</v>
       </c>
       <c r="H162">
-        <v>2</v>
+        <v>0.5636363636363636</v>
       </c>
       <c r="I162">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J162">
-        <v>2</v>
+        <v>-0.52801515151515155</v>
       </c>
       <c r="K162">
-        <v>2</v>
+        <v>-0.31</v>
       </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
@@ -6050,16 +6050,16 @@
         <v>3</v>
       </c>
       <c r="H163">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I163">
-        <v>2</v>
+        <v>0.35064935064935066</v>
       </c>
       <c r="J163">
-        <v>2</v>
+        <v>-0.27</v>
       </c>
       <c r="K163">
-        <v>2</v>
+        <v>-5.8181818181818182E-2</v>
       </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
@@ -6085,16 +6085,16 @@
         <v>4</v>
       </c>
       <c r="H164">
-        <v>2</v>
+        <v>0.10091717394249516</v>
       </c>
       <c r="I164">
-        <v>2</v>
+        <v>0.24237671841107397</v>
       </c>
       <c r="J164">
-        <v>2</v>
+        <v>4.3611012963478336E-2</v>
       </c>
       <c r="K164">
-        <v>2</v>
+        <v>-0.28574553180837764</v>
       </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
@@ -6680,16 +6680,16 @@
         <v>1</v>
       </c>
       <c r="H181">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I181">
         <v>0</v>
       </c>
       <c r="J181">
-        <v>-0.34893588236236184</v>
+        <v>-0.37457475889333491</v>
       </c>
       <c r="K181">
-        <v>2.7518472121991779E-3</v>
+        <v>0.12143282966219061</v>
       </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
@@ -6715,16 +6715,16 @@
         <v>2</v>
       </c>
       <c r="H182">
-        <v>8.5047290949930868E-2</v>
+        <v>1.4054593061539892E-2</v>
       </c>
       <c r="I182">
-        <v>2.6113544193652739E-2</v>
+        <v>0.85604925792714548</v>
       </c>
       <c r="J182">
-        <v>-2.7528898239636925E-3</v>
+        <v>-0.23257204604916282</v>
       </c>
       <c r="K182">
-        <v>-0.36154018455331122</v>
+        <v>-0.71597795257507768</v>
       </c>
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
@@ -7380,16 +7380,16 @@
         <v>1</v>
       </c>
       <c r="H201">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I201">
         <v>0</v>
       </c>
       <c r="J201">
-        <v>-0.34893588236236184</v>
+        <v>-0.3752649865433656</v>
       </c>
       <c r="K201">
-        <v>-0.2175645011465491</v>
+        <v>-0.37457475889333491</v>
       </c>
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
@@ -8080,16 +8080,16 @@
         <v>1</v>
       </c>
       <c r="H221">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I221">
         <v>0</v>
       </c>
       <c r="J221">
-        <v>-0.43788084950529738</v>
+        <v>-0.87196280274892179</v>
       </c>
       <c r="K221">
-        <v>-0.34893588236236184</v>
+        <v>-0.37457475889333491</v>
       </c>
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
@@ -8780,16 +8780,16 @@
         <v>1</v>
       </c>
       <c r="H241">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I241">
         <v>0</v>
       </c>
       <c r="J241">
-        <v>-0.34893588236236184</v>
+        <v>-0.37457475889333491</v>
       </c>
       <c r="K241">
-        <v>0.18430895950995158</v>
+        <v>0.24090096764279695</v>
       </c>
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.25">
@@ -8815,16 +8815,16 @@
         <v>2</v>
       </c>
       <c r="H242">
-        <v>1.2047143456321517E-2</v>
+        <v>8.190082643362552E-3</v>
       </c>
       <c r="I242">
-        <v>0.66019255567923552</v>
+        <v>0.86405829838606485</v>
       </c>
       <c r="J242">
-        <v>-0.19133971978128456</v>
+        <v>-0.39742046332864855</v>
       </c>
       <c r="K242">
-        <v>-0.78902202371103591</v>
+        <v>-0.72886307096447533</v>
       </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
@@ -9480,16 +9480,16 @@
         <v>1</v>
       </c>
       <c r="H261">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I261">
         <v>0</v>
       </c>
       <c r="J261">
-        <v>-0.34893588236236184</v>
+        <v>-0.37457475889333491</v>
       </c>
       <c r="K261">
-        <v>-3.6007388848796708E-2</v>
+        <v>-0.25579684856275925</v>
       </c>
     </row>
     <row r="262" spans="1:11" x14ac:dyDescent="0.25">
@@ -9515,16 +9515,16 @@
         <v>2</v>
       </c>
       <c r="H262">
-        <v>2</v>
+        <v>0.35718193429070177</v>
       </c>
       <c r="I262">
-        <v>2</v>
+        <v>0.17588240958120055</v>
       </c>
       <c r="J262">
-        <v>2</v>
+        <v>7.3487730922711852E-2</v>
       </c>
       <c r="K262">
-        <v>2</v>
+        <v>-0.46881736216402869</v>
       </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
@@ -9550,16 +9550,16 @@
         <v>3</v>
       </c>
       <c r="H263">
-        <v>2</v>
+        <v>5.6338803743778636E-2</v>
       </c>
       <c r="I263">
-        <v>2</v>
+        <v>0.55274032882531998</v>
       </c>
       <c r="J263">
-        <v>2</v>
+        <v>-0.13400022681184007</v>
       </c>
       <c r="K263">
-        <v>2</v>
+        <v>-0.54091179000333467</v>
       </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
@@ -10180,16 +10180,16 @@
         <v>1</v>
       </c>
       <c r="H281">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I281">
         <v>0</v>
       </c>
       <c r="J281">
-        <v>-0.34893588236236184</v>
+        <v>-0.7524946647683155</v>
       </c>
       <c r="K281">
-        <v>-0.25632373720754498</v>
+        <v>-0.37457475889333491</v>
       </c>
     </row>
     <row r="282" spans="1:11" x14ac:dyDescent="0.25">
@@ -10880,16 +10880,16 @@
         <v>1</v>
       </c>
       <c r="H301">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I301">
         <v>0</v>
       </c>
       <c r="J301">
-        <v>-0.34893588236236184</v>
+        <v>-0.37457475889333491</v>
       </c>
       <c r="K301">
-        <v>0.36586607180770397</v>
+        <v>0.3603691056234033</v>
       </c>
     </row>
     <row r="302" spans="1:11" x14ac:dyDescent="0.25">
@@ -10915,16 +10915,16 @@
         <v>2</v>
       </c>
       <c r="H302">
-        <v>6.3987880227127569E-3</v>
+        <v>5.7775208149282529E-3</v>
       </c>
       <c r="I302">
-        <v>0.79538463098954537</v>
+        <v>0.86734929860586163</v>
       </c>
       <c r="J302">
-        <v>-0.37912191969445125</v>
+        <v>-0.54593946902021795</v>
       </c>
       <c r="K302">
-        <v>-0.90146292110704618</v>
+        <v>-0.75649152733887126</v>
       </c>
     </row>
     <row r="303" spans="1:11" x14ac:dyDescent="0.25">
@@ -11580,16 +11580,16 @@
         <v>1</v>
       </c>
       <c r="H321">
-        <v>9.2214438511238006E-2</v>
+        <v>0.49138977797522593</v>
       </c>
       <c r="I321">
-        <v>0</v>
+        <v>6.1665080856140607E-2</v>
       </c>
       <c r="J321">
-        <v>-0.34893588236236184</v>
+        <v>7.3443561576728211E-2</v>
       </c>
       <c r="K321">
-        <v>0.1455497234489557</v>
+        <v>-0.44370276450765261</v>
       </c>
     </row>
     <row r="322" spans="1:11" x14ac:dyDescent="0.25">
@@ -11615,16 +11615,16 @@
         <v>2</v>
       </c>
       <c r="H322">
-        <v>3.1665738221864963E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I322">
-        <v>0.36391306770844734</v>
+        <v>0</v>
       </c>
       <c r="J322">
-        <v>-0.15522377280378422</v>
+        <v>-0.37457475889333491</v>
       </c>
       <c r="K322">
-        <v>-0.59655639658416426</v>
+        <v>-0.1363287105821529</v>
       </c>
     </row>
     <row r="323" spans="1:11" x14ac:dyDescent="0.25">
@@ -11650,16 +11650,16 @@
         <v>3</v>
       </c>
       <c r="H323">
-        <v>2</v>
+        <v>3.2480903996052142E-2</v>
       </c>
       <c r="I323">
-        <v>2</v>
+        <v>0.58592046307365675</v>
       </c>
       <c r="J323">
-        <v>2</v>
+        <v>-0.25806506176367172</v>
       </c>
       <c r="K323">
-        <v>2</v>
+        <v>-0.56153917542604093</v>
       </c>
     </row>
     <row r="324" spans="1:11" x14ac:dyDescent="0.25">
@@ -12280,16 +12280,16 @@
         <v>1</v>
       </c>
       <c r="H341">
-        <v>9.2214438511238006E-2</v>
+        <v>0.5973406899030318</v>
       </c>
       <c r="I341">
         <v>0</v>
       </c>
       <c r="J341">
-        <v>-0.34893588236236184</v>
+        <v>-0.6330265267877091</v>
       </c>
       <c r="K341">
-        <v>-7.4766624909792606E-2</v>
+        <v>-0.37457475889333491</v>
       </c>
     </row>
     <row r="342" spans="1:11" x14ac:dyDescent="0.25">
@@ -12980,16 +12980,16 @@
         <v>1</v>
       </c>
       <c r="H361">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I361">
         <v>0</v>
       </c>
       <c r="J361">
-        <v>-0.65597732430321098</v>
+        <v>-0.5764167329285298</v>
       </c>
       <c r="K361">
-        <v>7.4923580071964402E-4</v>
+        <v>5.2564028039120696E-4</v>
       </c>
     </row>
     <row r="362" spans="1:11" x14ac:dyDescent="0.25">
@@ -13015,16 +13015,16 @@
         <v>2</v>
       </c>
       <c r="H362">
-        <v>0.26602411252713715</v>
+        <v>7.2452600581458609E-2</v>
       </c>
       <c r="I362">
-        <v>9.9911799717462609E-3</v>
+        <v>0.79694228007414414</v>
       </c>
       <c r="J362">
-        <v>-7.5799715458296497E-4</v>
+        <v>-0.1665252039688398</v>
       </c>
       <c r="K362">
-        <v>-0.65826067680012212</v>
+        <v>-0.87233069437604938</v>
       </c>
     </row>
     <row r="363" spans="1:11" x14ac:dyDescent="0.25">
@@ -13680,16 +13680,16 @@
         <v>1</v>
       </c>
       <c r="H381">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I381">
         <v>0</v>
       </c>
       <c r="J381">
-        <v>-0.65597732430321098</v>
+        <v>-0.62610633177316288</v>
       </c>
       <c r="K381">
-        <v>-0.27372833878411296</v>
+        <v>-0.5764167329285298</v>
       </c>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.25">
@@ -14380,16 +14380,16 @@
         <v>1</v>
       </c>
       <c r="H401">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I401">
         <v>0</v>
       </c>
       <c r="J401">
-        <v>-0.65597732430321098</v>
+        <v>-1.252738303826717</v>
       </c>
       <c r="K401">
-        <v>-0.54820591336894553</v>
+        <v>-0.5764167329285298</v>
       </c>
     </row>
     <row r="402" spans="1:11" x14ac:dyDescent="0.25">
@@ -15080,16 +15080,16 @@
         <v>1</v>
       </c>
       <c r="H421">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I421">
         <v>0</v>
       </c>
       <c r="J421">
-        <v>-0.65597732430321098</v>
+        <v>-0.5764167329285298</v>
       </c>
       <c r="K421">
-        <v>0.14648063138195402</v>
+        <v>0.13669231899466935</v>
       </c>
     </row>
     <row r="422" spans="1:11" x14ac:dyDescent="0.25">
@@ -15115,16 +15115,16 @@
         <v>2</v>
       </c>
       <c r="H422">
-        <v>5.6274692304159338E-2</v>
+        <v>3.8704818566731032E-2</v>
       </c>
       <c r="I422">
-        <v>0.63553493713635256</v>
+        <v>0.84127586420551004</v>
       </c>
       <c r="J422">
-        <v>-0.16434701370041205</v>
+        <v>-0.32686962669179725</v>
       </c>
       <c r="K422">
-        <v>-0.9477882293127875</v>
+        <v>-0.90607257374453321</v>
       </c>
     </row>
     <row r="423" spans="1:11" x14ac:dyDescent="0.25">
@@ -15780,16 +15780,16 @@
         <v>1</v>
       </c>
       <c r="H441">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I441">
         <v>0</v>
       </c>
       <c r="J441">
-        <v>-0.65597732430321098</v>
+        <v>-0.5764167329285298</v>
       </c>
       <c r="K441">
-        <v>-0.12799694320287858</v>
+        <v>-0.48993965305888471</v>
       </c>
     </row>
     <row r="442" spans="1:11" x14ac:dyDescent="0.25">
@@ -16480,16 +16480,16 @@
         <v>1</v>
       </c>
       <c r="H461">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I461">
         <v>0</v>
       </c>
       <c r="J461">
-        <v>-0.65597732430321098</v>
+        <v>-1.1165716251124387</v>
       </c>
       <c r="K461">
-        <v>-0.40247451778771115</v>
+        <v>-0.5764167329285298</v>
       </c>
     </row>
     <row r="462" spans="1:11" x14ac:dyDescent="0.25">
@@ -17180,16 +17180,16 @@
         <v>1</v>
       </c>
       <c r="H481">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I481">
         <v>0</v>
       </c>
       <c r="J481">
-        <v>-0.65597732430321098</v>
+        <v>-0.5764167329285298</v>
       </c>
       <c r="K481">
-        <v>0.29221202696318838</v>
+        <v>0.2728589977089475</v>
       </c>
     </row>
     <row r="482" spans="1:11" x14ac:dyDescent="0.25">
@@ -17215,16 +17215,16 @@
         <v>2</v>
       </c>
       <c r="H482">
-        <v>3.0937657316659917E-2</v>
+        <v>2.6428259662552502E-2</v>
       </c>
       <c r="I482">
-        <v>0.7775273476061747</v>
+        <v>0.8573374060215343</v>
       </c>
       <c r="J482">
-        <v>-0.32134228382921565</v>
+        <v>-0.47280735922320627</v>
       </c>
       <c r="K482">
-        <v>-1.0731994176310755</v>
+        <v>-0.94411780536479395</v>
       </c>
     </row>
     <row r="483" spans="1:11" x14ac:dyDescent="0.25">
@@ -17880,16 +17880,16 @@
         <v>1</v>
       </c>
       <c r="H501">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I501">
         <v>0</v>
       </c>
       <c r="J501">
-        <v>-0.65597732430321098</v>
+        <v>-0.5764167329285298</v>
       </c>
       <c r="K501">
-        <v>1.7734452378355796E-2</v>
+        <v>-0.35377297434460658</v>
       </c>
     </row>
     <row r="502" spans="1:11" x14ac:dyDescent="0.25">
@@ -17915,16 +17915,16 @@
         <v>2</v>
       </c>
       <c r="H502">
-        <v>0.2033089069465025</v>
+        <v>0.1798506316634218</v>
       </c>
       <c r="I502">
-        <v>0.14116438413417873</v>
+        <v>0.46188740441818177</v>
       </c>
       <c r="J502">
-        <v>-2.4441220327510418E-2</v>
+        <v>-9.5486163342915042E-2</v>
       </c>
       <c r="K502">
-        <v>-0.73880063284673292</v>
+        <v>-0.77048460752793968</v>
       </c>
     </row>
     <row r="503" spans="1:11" x14ac:dyDescent="0.25">
@@ -17950,16 +17950,16 @@
         <v>3</v>
       </c>
       <c r="H503">
-        <v>2</v>
+        <v>0.39600950757383296</v>
       </c>
       <c r="I503">
-        <v>2</v>
+        <v>0.2160790554864547</v>
       </c>
       <c r="J503">
-        <v>2</v>
+        <v>6.7770160848925828E-2</v>
       </c>
       <c r="K503">
-        <v>2</v>
+        <v>-0.7241445001654897</v>
       </c>
     </row>
     <row r="504" spans="1:11" x14ac:dyDescent="0.25">
@@ -18580,16 +18580,16 @@
         <v>1</v>
       </c>
       <c r="H521">
-        <v>0.27134302209382816</v>
+        <v>0.68083339357139072</v>
       </c>
       <c r="I521">
         <v>0</v>
       </c>
       <c r="J521">
-        <v>-0.65597732430321098</v>
+        <v>-0.98040494639816067</v>
       </c>
       <c r="K521">
-        <v>-0.25674312220647677</v>
+        <v>-0.5764167329285298</v>
       </c>
     </row>
     <row r="522" spans="1:11" x14ac:dyDescent="0.25">
@@ -19280,16 +19280,16 @@
         <v>1</v>
       </c>
       <c r="H541">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I541">
         <v>0</v>
       </c>
       <c r="J541">
-        <v>-0.92196800378321153</v>
+        <v>-0.77860452092188626</v>
       </c>
       <c r="K541">
-        <v>-9.0980984654621365E-3</v>
+        <v>-0.1096433924808449</v>
       </c>
     </row>
     <row r="542" spans="1:11" x14ac:dyDescent="0.25">
@@ -19315,16 +19315,16 @@
         <v>2</v>
       </c>
       <c r="H542">
-        <v>2</v>
+        <v>0.60948393108753462</v>
       </c>
       <c r="I542">
-        <v>2</v>
+        <v>0.13710955477981554</v>
       </c>
       <c r="J542">
-        <v>2</v>
+        <v>5.1606339858017769E-2</v>
       </c>
       <c r="K542">
-        <v>2</v>
+        <v>-0.8817342318416439</v>
       </c>
     </row>
     <row r="543" spans="1:11" x14ac:dyDescent="0.25">
@@ -19350,16 +19350,16 @@
         <v>3</v>
       </c>
       <c r="H543">
-        <v>2</v>
+        <v>0.15445079116280253</v>
       </c>
       <c r="I543">
-        <v>2</v>
+        <v>0.71201511948914586</v>
       </c>
       <c r="J543">
-        <v>2</v>
+        <v>-0.10706265495861109</v>
       </c>
       <c r="K543">
-        <v>2</v>
+        <v>-1.0388946849950589</v>
       </c>
     </row>
     <row r="544" spans="1:11" x14ac:dyDescent="0.25">
@@ -19980,16 +19980,16 @@
         <v>1</v>
       </c>
       <c r="H561">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I561">
         <v>0</v>
       </c>
       <c r="J561">
-        <v>-0.92196800378321153</v>
+        <v>-0.87781194286496411</v>
       </c>
       <c r="K561">
-        <v>-0.33597705999574934</v>
+        <v>-0.77860452092188626</v>
       </c>
     </row>
     <row r="562" spans="1:11" x14ac:dyDescent="0.25">
@@ -20680,16 +20680,16 @@
         <v>1</v>
       </c>
       <c r="H581">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I581">
         <v>0</v>
       </c>
       <c r="J581">
-        <v>-0.92196800378321153</v>
+        <v>-1.6459804932490834</v>
       </c>
       <c r="K581">
-        <v>-0.66285602152603662</v>
+        <v>-0.77860452092188626</v>
       </c>
     </row>
     <row r="582" spans="1:11" x14ac:dyDescent="0.25">
@@ -21380,16 +21380,16 @@
         <v>1</v>
       </c>
       <c r="H601">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I601">
         <v>0</v>
       </c>
       <c r="J601">
-        <v>-0.92196800378321153</v>
+        <v>-0.77860452092188626</v>
       </c>
       <c r="K601">
-        <v>0.11327135539213576</v>
+        <v>3.8284702232225333E-2</v>
       </c>
     </row>
     <row r="602" spans="1:11" x14ac:dyDescent="0.25">
@@ -21415,16 +21415,16 @@
         <v>2</v>
       </c>
       <c r="H602">
-        <v>0.10481926310346126</v>
+        <v>7.2610246384500657E-2</v>
       </c>
       <c r="I602">
-        <v>0.60667186428609521</v>
+        <v>0.81564111111304838</v>
       </c>
       <c r="J602">
-        <v>-0.13976903180078798</v>
+        <v>-0.27807844546934513</v>
       </c>
       <c r="K602">
-        <v>-1.1318044896848631</v>
+        <v>-1.088131425556744</v>
       </c>
     </row>
     <row r="603" spans="1:11" x14ac:dyDescent="0.25">
@@ -22080,16 +22080,16 @@
         <v>1</v>
       </c>
       <c r="H621">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I621">
         <v>0</v>
       </c>
       <c r="J621">
-        <v>-0.92196800378321153</v>
+        <v>-0.77860452092188626</v>
       </c>
       <c r="K621">
-        <v>-0.21360760613815144</v>
+        <v>-0.72988384815189389</v>
       </c>
     </row>
     <row r="622" spans="1:11" x14ac:dyDescent="0.25">
@@ -22780,16 +22780,16 @@
         <v>1</v>
       </c>
       <c r="H641">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I641">
         <v>0</v>
       </c>
       <c r="J641">
-        <v>-0.92196800378321153</v>
+        <v>-1.4980523985360132</v>
       </c>
       <c r="K641">
-        <v>-0.54048656766843872</v>
+        <v>-0.77860452092188626</v>
       </c>
     </row>
     <row r="642" spans="1:11" x14ac:dyDescent="0.25">
@@ -23480,16 +23480,16 @@
         <v>1</v>
       </c>
       <c r="H661">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I661">
         <v>0</v>
       </c>
       <c r="J661">
-        <v>-0.92196800378321153</v>
+        <v>-0.77860452092188626</v>
       </c>
       <c r="K661">
-        <v>0.23564080924973366</v>
+        <v>0.18621279694529555</v>
       </c>
     </row>
     <row r="662" spans="1:11" x14ac:dyDescent="0.25">
@@ -23515,16 +23515,16 @@
         <v>2</v>
       </c>
       <c r="H662">
-        <v>5.9536476201732337E-2</v>
+        <v>4.7839372210576422E-2</v>
       </c>
       <c r="I662">
-        <v>0.75637994032949141</v>
+        <v>0.84682996505997088</v>
       </c>
       <c r="J662">
-        <v>-0.27525304368744918</v>
+        <v>-0.43162896119252248</v>
       </c>
       <c r="K662">
-        <v>-1.2609672031595003</v>
+        <v>-1.1272248846482587</v>
       </c>
     </row>
     <row r="663" spans="1:11" x14ac:dyDescent="0.25">
@@ -24180,16 +24180,16 @@
         <v>1</v>
       </c>
       <c r="H681">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I681">
         <v>0</v>
       </c>
       <c r="J681">
-        <v>-0.92196800378321153</v>
+        <v>-0.77860452092188626</v>
       </c>
       <c r="K681">
-        <v>-9.1238152280553556E-2</v>
+        <v>-0.58195575343882366</v>
       </c>
     </row>
     <row r="682" spans="1:11" x14ac:dyDescent="0.25">
@@ -24880,16 +24880,16 @@
         <v>1</v>
       </c>
       <c r="H701">
-        <v>0.38815273071201051</v>
+        <v>0.73964047356535112</v>
       </c>
       <c r="I701">
         <v>0</v>
       </c>
       <c r="J701">
-        <v>-0.92196800378321153</v>
+        <v>-1.3501243038229429</v>
       </c>
       <c r="K701">
-        <v>-0.41811711381084077</v>
+        <v>-0.77860452092188626</v>
       </c>
     </row>
     <row r="702" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>